<commit_message>
merged feature descirption of tables
</commit_message>
<xml_diff>
--- a/artifacts/feature_description.xlsx
+++ b/artifacts/feature_description.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
-  <si>
-    <t>Bank</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="178">
+  <si>
+    <t>Bank &amp; Cibil data</t>
   </si>
   <si>
     <t>Variable Name</t>
@@ -25,7 +25,16 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Internal</t>
+    <t>51336 Customers</t>
+  </si>
+  <si>
+    <t>PROSPECTID</t>
+  </si>
+  <si>
+    <t>Customer masked unique ID</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Total_TL</t>
@@ -178,21 +187,12 @@
     <t>Age of newest opened account</t>
   </si>
   <si>
-    <t xml:space="preserve">Cibil </t>
-  </si>
-  <si>
-    <t>External</t>
-  </si>
-  <si>
     <t>time_since_recent_payment</t>
   </si>
   <si>
     <t>Time Since recent Payment made</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>time_since_first_deliquency</t>
   </si>
   <si>
@@ -539,6 +539,9 @@
   </si>
   <si>
     <t>Applicant's credit score</t>
+  </si>
+  <si>
+    <t>Target Feature</t>
   </si>
   <si>
     <t>Approved_Flag</t>
@@ -911,7 +914,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -933,8 +936,8 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -944,782 +947,788 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2"/>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="A28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="2"/>
       <c r="B57" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="2"/>
       <c r="B58" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="2"/>
       <c r="B59" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="2"/>
       <c r="B60" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="2"/>
       <c r="B61" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="2"/>
       <c r="B63" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="2"/>
       <c r="B64" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="2"/>
       <c r="B65" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="2"/>
       <c r="B66" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="2"/>
       <c r="B67" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="2"/>
       <c r="B68" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>136</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C68" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="2"/>
       <c r="B69" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C69" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="2"/>
       <c r="B70" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C70" s="2"/>
+        <v>139</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="2"/>
       <c r="B71" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="2"/>
       <c r="B72" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="2"/>
       <c r="B73" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="2"/>
       <c r="B74" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="2"/>
       <c r="B75" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="2"/>
       <c r="B76" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="2"/>
       <c r="B77" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="2"/>
       <c r="B78" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="2"/>
       <c r="B79" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="2"/>
       <c r="B80" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="2"/>
       <c r="B81" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="2"/>
       <c r="B82" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="2"/>
       <c r="B83" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="2"/>
       <c r="B84" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="2"/>
       <c r="B85" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="2"/>
       <c r="B86" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="2"/>
       <c r="B87" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
-      <c r="A88" s="2"/>
+      <c r="A88" s="2" t="s">
+        <v>175</v>
+      </c>
       <c r="B88" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="2"/>
-      <c r="B89" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>176</v>
-      </c>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="2"/>
@@ -1736,11 +1745,6 @@
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
-      <c r="A93" s="2"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>